<commit_message>
Made movement card loader more effcient
</commit_message>
<xml_diff>
--- a/BotCode/RobotBOM.xlsx
+++ b/BotCode/RobotBOM.xlsx
@@ -1,8 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x15 xr">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="7A36849440CDCF6CC15FC52FB9B2C898B1406C6A"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="120" windowWidth="20730" windowHeight="10035"/>
   </bookViews>
@@ -11,12 +12,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162912"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="55">
   <si>
     <t>Item</t>
   </si>
@@ -159,7 +160,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
@@ -315,7 +316,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -350,7 +351,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -558,21 +559,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac xr" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="25.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="122.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="100.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -590,7 +591,7 @@
       </c>
       <c r="F1" s="3"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
@@ -609,7 +610,7 @@
       </c>
       <c r="F2" s="3"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
@@ -628,7 +629,7 @@
       </c>
       <c r="F3" s="3"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
@@ -647,7 +648,7 @@
       </c>
       <c r="F4" s="3"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
@@ -666,7 +667,7 @@
       </c>
       <c r="F5" s="3"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>38</v>
       </c>
@@ -685,7 +686,7 @@
       </c>
       <c r="F6" s="3"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>13</v>
       </c>
@@ -704,7 +705,7 @@
       </c>
       <c r="F7" s="3"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>34</v>
       </c>
@@ -723,7 +724,7 @@
       </c>
       <c r="F8" s="3"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>15</v>
       </c>
@@ -742,7 +743,7 @@
       </c>
       <c r="F9" s="3"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>22</v>
       </c>
@@ -763,7 +764,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>17</v>
       </c>
@@ -782,7 +783,7 @@
       </c>
       <c r="F11" s="3"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>19</v>
       </c>
@@ -801,7 +802,7 @@
       </c>
       <c r="F12" s="3"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>31</v>
       </c>
@@ -820,7 +821,7 @@
       </c>
       <c r="F13" s="3"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>40</v>
       </c>
@@ -839,7 +840,7 @@
       </c>
       <c r="F14" s="3"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>21</v>
       </c>
@@ -858,7 +859,7 @@
       </c>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>24</v>
       </c>
@@ -879,7 +880,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>26</v>
       </c>
@@ -900,7 +901,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>29</v>
       </c>
@@ -921,7 +922,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>44</v>
       </c>
@@ -942,7 +943,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -962,24 +963,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac xr" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac xr" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fixed bugs in player shutdown and move submission code.
</commit_message>
<xml_diff>
--- a/BotCode/RobotBOM.xlsx
+++ b/BotCode/RobotBOM.xlsx
@@ -87,12 +87,6 @@
     <t>Wheels</t>
   </si>
   <si>
-    <t>Caster 3/8"</t>
-  </si>
-  <si>
-    <t>Any caster will work, like this one: http://www.robotshop.com/en/pololu-ball-caster-1-2-in-plastic-ball.html</t>
-  </si>
-  <si>
     <t>LED Driver</t>
   </si>
   <si>
@@ -120,9 +114,6 @@
     <t>9-DOF Board</t>
   </si>
   <si>
-    <t>https://www.adafruit.com/products/2021</t>
-  </si>
-  <si>
     <t>https://www.adafruit.com/products/2744</t>
   </si>
   <si>
@@ -150,10 +141,19 @@
     <t>Several of these is a good idea</t>
   </si>
   <si>
-    <t>https://www.pololu.com/product/950</t>
-  </si>
-  <si>
     <t>https://www.pololu.com/product/2820</t>
+  </si>
+  <si>
+    <t>https://www.adafruit.com/products/1714</t>
+  </si>
+  <si>
+    <t>Caster 1"</t>
+  </si>
+  <si>
+    <t>https://www.pololu.com/product/2691</t>
+  </si>
+  <si>
+    <t>Any caster will work, like this one: https://www.pololu.com/product/952</t>
   </si>
 </sst>
 </file>
@@ -235,7 +235,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -247,6 +247,7 @@
     <xf numFmtId="44" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -556,8 +557,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -665,10 +666,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C6" s="2">
         <v>1</v>
@@ -703,10 +704,10 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="C8" s="2">
         <v>1</v>
@@ -744,7 +745,7 @@
         <v>22</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C10" s="2">
         <v>2</v>
@@ -757,7 +758,7 @@
         <v>5</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -800,10 +801,10 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C13" s="2">
         <v>1</v>
@@ -819,10 +820,10 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C14" s="2">
         <v>1</v>
@@ -836,12 +837,12 @@
       </c>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C15" s="2">
         <v>2</v>
@@ -855,33 +856,33 @@
       </c>
       <c r="F15" s="7"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B16" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" t="s">
         <v>44</v>
       </c>
       <c r="C16" s="2">
         <v>1</v>
       </c>
-      <c r="D16" s="4">
-        <v>1.99</v>
+      <c r="D16" s="9">
+        <v>3.95</v>
       </c>
       <c r="E16" s="4">
         <f>D16*C16</f>
-        <v>1.99</v>
+        <v>3.95</v>
       </c>
       <c r="F16" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="5" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>26</v>
       </c>
       <c r="C17" s="5">
         <v>1</v>
@@ -894,15 +895,15 @@
         <v>1.64</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C18" s="5">
         <v>1</v>
@@ -915,15 +916,15 @@
         <v>0.62</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C19" s="2">
         <v>1</v>
@@ -936,7 +937,7 @@
         <v>0.1</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -944,11 +945,11 @@
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E20" s="8">
         <f>SUM(E2:E19)</f>
-        <v>85.600000000000009</v>
+        <v>87.560000000000016</v>
       </c>
       <c r="F20" s="2"/>
     </row>

</xml_diff>

<commit_message>
Updates to robot code, fixes for game sounds and new sounds, UI fixes.
</commit_message>
<xml_diff>
--- a/BotCode/RobotBOM.xlsx
+++ b/BotCode/RobotBOM.xlsx
@@ -567,7 +567,7 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -860,7 +860,7 @@
         <v>4.95</v>
       </c>
       <c r="E15" s="4">
-        <f>D15*C15</f>
+        <f t="shared" ref="E15:E20" si="3">D15*C15</f>
         <v>9.9</v>
       </c>
       <c r="F15" s="7"/>
@@ -879,7 +879,7 @@
         <v>3.95</v>
       </c>
       <c r="E16" s="4">
-        <f>D16*C16</f>
+        <f t="shared" si="3"/>
         <v>3.95</v>
       </c>
       <c r="F16" s="2" t="s">
@@ -900,7 +900,7 @@
         <v>1.64</v>
       </c>
       <c r="E17" s="6">
-        <f>D17*C17</f>
+        <f t="shared" si="3"/>
         <v>1.64</v>
       </c>
       <c r="F17" s="2" t="s">
@@ -921,7 +921,7 @@
         <v>0.62</v>
       </c>
       <c r="E18" s="6">
-        <f>D18*C18</f>
+        <f t="shared" si="3"/>
         <v>0.62</v>
       </c>
       <c r="F18" s="2" t="s">
@@ -942,7 +942,7 @@
         <v>0.1</v>
       </c>
       <c r="E19" s="4">
-        <f>D19*C19</f>
+        <f t="shared" si="3"/>
         <v>0.1</v>
       </c>
       <c r="F19" s="2" t="s">
@@ -963,7 +963,7 @@
         <v>10.1</v>
       </c>
       <c r="E20" s="4">
-        <f>D20*C20</f>
+        <f t="shared" si="3"/>
         <v>10.1</v>
       </c>
       <c r="F20" s="2" t="s">

</xml_diff>